<commit_message>
feature: parse operations from .xlsx file
</commit_message>
<xml_diff>
--- a/src/main/resources/dev/operaciones.xlsx
+++ b/src/main/resources/dev/operaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\IdeaProjects\parser-excel\src\main\resources\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\IdeaProjects\OperationsManager\src\main\resources\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D7045A-F706-416B-9BEB-0DEA2A85D1D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589059C7-A806-4446-B00F-534A0009E0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" tabRatio="677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" tabRatio="677" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Llegadas" sheetId="5" r:id="rId1"/>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>AERONAVES GRAN TAMAÑO</t>
   </si>
   <si>
     <t>PUBLICO</t>
-  </si>
-  <si>
-    <t>396 890</t>
   </si>
   <si>
     <t>18/36</t>
@@ -385,10 +382,19 @@
     <t>CAT ESTELA AERONAVE</t>
   </si>
   <si>
-    <t xml:space="preserve">LFPO </t>
-  </si>
-  <si>
     <t>UUDD</t>
+  </si>
+  <si>
+    <t>16:00H</t>
+  </si>
+  <si>
+    <t>16:26H</t>
+  </si>
+  <si>
+    <t>16:46H</t>
+  </si>
+  <si>
+    <t>LFPO</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="hh:mm&quot;H&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -661,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -686,12 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -741,6 +741,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -777,13 +790,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1159,10 +1171,10 @@
   </sheetPr>
   <dimension ref="A1:T1046124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1170,7 +1182,7 @@
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" customWidth="1"/>
     <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13" style="23" customWidth="1"/>
+    <col min="4" max="4" width="13" style="21" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.109375" customWidth="1"/>
@@ -1178,7 +1190,7 @@
     <col min="9" max="9" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12.44140625" customWidth="1"/>
     <col min="14" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="15" width="14" style="23" customWidth="1"/>
+    <col min="15" max="15" width="14" style="21" customWidth="1"/>
     <col min="16" max="16" width="55.33203125" customWidth="1"/>
     <col min="17" max="17" width="56.109375" customWidth="1"/>
     <col min="18" max="18" width="10.109375" customWidth="1"/>
@@ -1186,147 +1198,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="28"/>
+      <c r="A1" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
+      <c r="A2" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="1:20" ht="55.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="43" t="s">
+        <v>13</v>
+      </c>
       <c r="G3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="40" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="43" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="35"/>
+        <v>25</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="38"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="41"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="41"/>
+        <v>4</v>
+      </c>
+      <c r="H4" s="44"/>
       <c r="I4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="44"/>
+        <v>3</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="37"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="40"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" s="23" t="s">
         <v>45</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="T4" s="25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -1339,65 +1351,65 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <v>42511</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="9">
         <v>85100</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="11" t="s">
+      <c r="L5" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="11">
+      <c r="M5" s="9">
         <v>18</v>
       </c>
-      <c r="N5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="46"/>
+      <c r="N5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="35"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C12" s="23"/>
+      <c r="C12" s="21"/>
       <c r="D12"/>
-      <c r="N12" s="23"/>
+      <c r="N12" s="21"/>
       <c r="O12"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13"/>
-      <c r="N13" s="23"/>
+      <c r="N13" s="21"/>
       <c r="O13"/>
     </row>
     <row r="19" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L19" s="47"/>
+      <c r="L19" s="31"/>
     </row>
     <row r="1046124" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O1046124" s="32"/>
+      <c r="O1046124" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1445,10 +1457,10 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1463,149 +1475,149 @@
     <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="12" width="11.5546875"/>
-    <col min="13" max="13" width="11.44140625" style="23"/>
+    <col min="13" max="13" width="11.44140625" style="21"/>
     <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="58.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="56.109375" style="16" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="29.88671875" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="11.44140625" style="16"/>
+    <col min="16" max="16" width="56.109375" style="14" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="29.88671875" style="14" customWidth="1"/>
+    <col min="19" max="16384" width="11.44140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="28"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="23.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="31"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="43" t="s">
+        <v>13</v>
+      </c>
       <c r="G3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="40" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="43" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="40" t="s">
+      <c r="M3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="35"/>
+      <c r="N3" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="38"/>
     </row>
     <row r="4" spans="1:19" ht="26.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="41"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="41"/>
+        <v>4</v>
+      </c>
+      <c r="H4" s="44"/>
       <c r="I4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="44"/>
+        <v>3</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="40"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="23" t="s">
         <v>45</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="S4" s="25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1622,40 +1634,40 @@
         <v>42034</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <v>396890</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="9">
-        <v>0.66666666666666674</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0.68472222222222223</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0.69861111111111107</v>
-      </c>
-      <c r="M5" s="22">
+      <c r="K5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="20">
         <v>36</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="46"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
feature: added initial chart view and control
</commit_message>
<xml_diff>
--- a/src/main/resources/dev/operaciones.xlsx
+++ b/src/main/resources/dev/operaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\IdeaProjects\OperationsManager\src\main\resources\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589059C7-A806-4446-B00F-534A0009E0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A4DD34-E97B-4B91-8815-491DC1F3439D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" tabRatio="677" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" tabRatio="677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Llegadas" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -402,7 +404,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -667,12 +669,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,11 +741,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,12 +793,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1171,10 +1170,10 @@
   </sheetPr>
   <dimension ref="A1:T1046124"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1182,7 +1181,7 @@
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" customWidth="1"/>
     <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13" style="21" customWidth="1"/>
+    <col min="4" max="4" width="13" style="20" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.109375" customWidth="1"/>
@@ -1190,7 +1189,7 @@
     <col min="9" max="9" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12.44140625" customWidth="1"/>
     <col min="14" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="15" width="14" style="21" customWidth="1"/>
+    <col min="15" max="15" width="14" style="20" customWidth="1"/>
     <col min="16" max="16" width="55.33203125" customWidth="1"/>
     <col min="17" max="17" width="56.109375" customWidth="1"/>
     <col min="18" max="18" width="10.109375" customWidth="1"/>
@@ -1198,146 +1197,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="26"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:20" ht="55.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="39"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="4" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="40"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="22" t="s">
+      <c r="O4" s="41"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="22" t="s">
+      <c r="S4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="T4" s="22" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1351,65 +1350,65 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>42511</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>85100</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>18</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="35"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="36"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12"/>
-      <c r="N12" s="21"/>
+      <c r="N12" s="20"/>
       <c r="O12"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C13" s="21"/>
+      <c r="C13" s="20"/>
       <c r="D13"/>
-      <c r="N13" s="21"/>
+      <c r="N13" s="20"/>
       <c r="O13"/>
     </row>
     <row r="19" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L19" s="31"/>
+      <c r="L19" s="30"/>
     </row>
     <row r="1046124" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O1046124" s="30"/>
+      <c r="O1046124" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1457,10 +1456,10 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1475,148 +1474,148 @@
     <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="12" width="11.5546875"/>
-    <col min="13" max="13" width="11.44140625" style="21"/>
+    <col min="13" max="13" width="11.44140625" style="20"/>
     <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="58.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="56.109375" style="14" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" style="14" customWidth="1"/>
-    <col min="18" max="18" width="29.88671875" style="14" customWidth="1"/>
-    <col min="19" max="16384" width="11.44140625" style="14"/>
+    <col min="16" max="16" width="56.109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="29.88671875" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="11.44140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="10" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="26"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:19" ht="23.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="29"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="28"/>
     </row>
     <row r="3" spans="1:19" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="26.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="4" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="22" t="s">
+      <c r="N4" s="41"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="22" t="s">
+      <c r="R4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="22" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1630,7 +1629,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="14">
         <v>42034</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1648,26 +1647,26 @@
       <c r="I5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="19">
         <v>36</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>